<commit_message>
Correction dans le journal de veille
Quelques erreures ont été corrigé.
</commit_message>
<xml_diff>
--- a/Doc/JournalDeVeille.xlsx
+++ b/Doc/JournalDeVeille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugop\Documents\1School1\Informatique\ProjetDApprofondissement1\Projet\Approfondissement1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49711450-8DE8-4E8E-933B-764BD977215D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6B92CD-6022-40A5-BFFB-3B433D382A07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{99D81F4C-E14F-475B-A89B-68D417F4CC95}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>Journal de veille technologique</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>Cette page présente l'utilisation de bootstrap avec les balises &lt;button&gt;, ainsi que les différentes apparences estéthique que ceux-ci peuvent avoir.</t>
+  </si>
+  <si>
+    <t>Hugo Proulx</t>
+  </si>
+  <si>
+    <t>DA: 1801324</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,8 +271,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -311,21 +329,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -343,6 +361,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,362 +813,379 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FC5144-D522-4A27-B795-CAA4CF26E9AA}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" customWidth="1"/>
+    <col min="6" max="6" width="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="4" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F4" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="5" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="6" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F6" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="7" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F7" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="8" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F8" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="9" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F9" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="10" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="11" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F11" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="12" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F12" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="13" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F13" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="14" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F14" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="15" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="16" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F16" s="14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="17" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F17" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="18" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F18" s="14" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" display="https://vuejs.org/v2/guide/list.html" xr:uid="{22B156C1-B8CC-49FD-BB8F-E271697DB888}"/>
-    <hyperlink ref="D7" r:id="rId2" display="https://stackoverflow.com/questions/46639068/display-only-a-part-of-the-name-if-characters-exceed-a-limit-in-vue-js" xr:uid="{D7A3F93C-199F-4FB2-9230-D2701C1EDC94}"/>
+    <hyperlink ref="D6" r:id="rId1" display="https://vuejs.org/v2/guide/list.html" xr:uid="{22B156C1-B8CC-49FD-BB8F-E271697DB888}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://stackoverflow.com/questions/46639068/display-only-a-part-of-the-name-if-characters-exceed-a-limit-in-vue-js" xr:uid="{D7A3F93C-199F-4FB2-9230-D2701C1EDC94}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <headerFooter>
+    <oddHeader>&amp;LHugo Proulx
+&amp;RDA:1801324</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>